<commit_message>
Added Test results excel file
</commit_message>
<xml_diff>
--- a/Test  Results.xlsx
+++ b/Test  Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8B5B3F-5EBF-46E2-8B57-6950BF8D7549}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A385333-DB3B-4739-B5D5-90735198CA93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="23">
   <si>
     <t>Method:</t>
   </si>
@@ -80,6 +80,21 @@
   <si>
     <t>TEST 5</t>
   </si>
+  <si>
+    <t>hasn't changed over multiple turns, one child in uniform, ROULETTE select, tournament replace:</t>
+  </si>
+  <si>
+    <t>TEST 6</t>
+  </si>
+  <si>
+    <t>hasn't changed over multiple turns, TWO child in ARITHRECOMB, tournament select, tournament replace:</t>
+  </si>
+  <si>
+    <t>hasn't changed over multiple turns, ONE child in uniform, tournament select, replaceWORST replace:</t>
+  </si>
+  <si>
+    <t>TEST 7</t>
+  </si>
 </sst>
 </file>
 
@@ -131,6 +146,3218 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$109</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Training Fitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$110:$A$120</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Average:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$110:$B$120</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>9.3402468402396494E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.78614211984813E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1655901457871997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6420958075981694E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.20872889416388E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3075143045881999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.16090302287098E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2944637917724097E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6378980862200399E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.84155212054853E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.538513513363719E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7B8D-4259-9C91-7E3ABBCFFD3F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$109</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test Fitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$110:$A$120</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Average:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$110:$C$120</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.207491974297737</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.8268714832012702E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8886354453305307E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20737843392390201</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.90952467500332E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0262377365511101E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.88031895885028E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.5607879460678794E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.4809600331596202E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.224378683920749</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1034982454924028</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7B8D-4259-9C91-7E3ABBCFFD3F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="448652127"/>
+        <c:axId val="459587519"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="448652127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="459587519"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="459587519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="448652127"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$91</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Training Fitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$92:$A$102</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Average:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$92:$B$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7.2716735001233698E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.103592529322325</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12682245271051501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9130402377585206E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.120834627713059</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1063588836462101E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12677107667388199</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9821073653700201E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1976442102352498E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.117654678798976</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.266048092979734E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CB2-4F88-A62E-06959542B750}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$91</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test Fitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$92:$A$102</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Average:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$92:$C$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.14175836252414101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23843350933772001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27992921620276001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23707512211589701</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26374140187835798</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11148833614487801</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.27479313725993498</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21416179252013201</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.6384267161555206E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.168758686868688</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.19397779915686644</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4CB2-4F88-A62E-06959542B750}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="108816959"/>
+        <c:axId val="454750991"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="108816959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="454750991"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="454750991"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="108816959"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$74</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Training Fitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$75:$A$85</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Average:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$75:$B$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.9097073958828198E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9458118086988896E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.84348463884215E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.69874339228349E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0216180339773001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2963198698327499E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5655196021955098E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.8527673780407898E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3222058603910901E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2475007857675901E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.770367876591238E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E22F-4345-BA1E-3773CBF77404}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$74</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test Fitness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$75:$A$85</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Average:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$75:$C$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.110245305644407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.165086018359449</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.124602628137528</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3508739254674706E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12134464855332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.3550771835034403E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.4738887039438102E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.13552208322409601</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8359866970224999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.78465581141482E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.348055071323203E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E22F-4345-BA1E-3773CBF77404}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="482091743"/>
+        <c:axId val="454553887"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="482091743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="454553887"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="454553887"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="482091743"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E74698BB-DD32-474C-8DC4-A3CC73AD2C19}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93FE8458-E16E-46D2-A38D-F69884203520}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F912C7C6-DF2A-4B70-A629-0673F0DEF669}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -396,10 +3623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,10 +3811,10 @@
         <v>1</v>
       </c>
       <c r="B23">
-        <v>0.09</v>
+        <v>3.8291110673301897E-2</v>
       </c>
       <c r="C23">
-        <v>0.21</v>
+        <v>0.126157978460465</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -627,31 +3854,67 @@
       <c r="A27">
         <v>5</v>
       </c>
+      <c r="B27">
+        <v>9.9943120413363895E-2</v>
+      </c>
+      <c r="C27">
+        <v>0.229379370515812</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
+      <c r="B28">
+        <v>3.5693758221029E-2</v>
+      </c>
+      <c r="C28">
+        <v>0.11164213217684101</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7</v>
       </c>
+      <c r="B29">
+        <v>0.11112800257984599</v>
+      </c>
+      <c r="C29">
+        <v>0.23954424544462399</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>8</v>
       </c>
+      <c r="B30">
+        <v>2.6196557574678599E-2</v>
+      </c>
+      <c r="C30">
+        <v>8.5666827098220794E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9</v>
       </c>
+      <c r="B31">
+        <v>2.9905354882376799E-2</v>
+      </c>
+      <c r="C31">
+        <v>0.19854631606070799</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>10</v>
       </c>
+      <c r="B32">
+        <v>1.35525008162338E-2</v>
+      </c>
+      <c r="C32">
+        <v>4.0005319956159899E-2</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -659,11 +3922,11 @@
       </c>
       <c r="B33">
         <f>AVERAGE(B23:B32)</f>
-        <v>7.3229555672966851E-2</v>
+        <v>5.5762862785269741E-2</v>
       </c>
       <c r="C33">
         <f>AVERAGE(C23:C32)</f>
-        <v>0.17966618737821974</v>
+        <v>0.15396069392257097</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -988,7 +4251,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1007,10 +4270,10 @@
         <v>1</v>
       </c>
       <c r="B75">
-        <v>2.9608954460630801E-2</v>
+        <v>2.9097073958828198E-2</v>
       </c>
       <c r="C75">
-        <v>0.11072085858403199</v>
+        <v>0.110245305644407</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1018,10 +4281,10 @@
         <v>2</v>
       </c>
       <c r="B76">
-        <v>1.06292830988239E-2</v>
-      </c>
-      <c r="C76" t="s">
-        <v>15</v>
+        <v>7.9458118086988896E-2</v>
+      </c>
+      <c r="C76">
+        <v>0.165086018359449</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1029,10 +4292,10 @@
         <v>3</v>
       </c>
       <c r="B77">
-        <v>4.1067827339811701E-2</v>
+        <v>4.84348463884215E-2</v>
       </c>
       <c r="C77">
-        <v>0.125438476831117</v>
+        <v>0.124602628137528</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1040,10 +4303,10 @@
         <v>4</v>
       </c>
       <c r="B78">
-        <v>1.4486382170940001E-2</v>
+        <v>2.69874339228349E-2</v>
       </c>
       <c r="C78">
-        <v>1.53241467045025E-2</v>
+        <v>6.3508739254674706E-2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1051,10 +4314,10 @@
         <v>5</v>
       </c>
       <c r="B79">
-        <v>7.6837967645025E-3</v>
+        <v>5.0216180339773001E-2</v>
       </c>
       <c r="C79">
-        <v>2.56786759338287E-2</v>
+        <v>0.12134464855332</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1062,10 +4325,10 @@
         <v>6</v>
       </c>
       <c r="B80">
-        <v>3.3595659887734802E-2</v>
+        <v>3.2963198698327499E-2</v>
       </c>
       <c r="C80">
-        <v>7.6673050845586704E-2</v>
+        <v>3.3550771835034403E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1073,10 +4336,10 @@
         <v>7</v>
       </c>
       <c r="B81">
-        <v>1.04569909902346E-2</v>
+        <v>3.5655196021955098E-2</v>
       </c>
       <c r="C81">
-        <v>1.6759291971967301E-2</v>
+        <v>3.4738887039438102E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1084,10 +4347,10 @@
         <v>8</v>
       </c>
       <c r="B82">
-        <v>7.93853128298329E-3</v>
+        <v>4.8527673780407898E-2</v>
       </c>
       <c r="C82">
-        <v>8.3339449710838898E-3</v>
+        <v>0.13552208322409601</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1095,10 +4358,10 @@
         <v>9</v>
       </c>
       <c r="B83">
-        <v>1.47459953579341E-2</v>
+        <v>1.3222058603910901E-2</v>
       </c>
       <c r="C83">
-        <v>3.0098670038499899E-2</v>
+        <v>2.8359866970224999E-2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1106,10 +4369,10 @@
         <v>10</v>
       </c>
       <c r="B84">
-        <v>9.5918094702410993E-3</v>
+        <v>1.2475007857675901E-2</v>
       </c>
       <c r="C84">
-        <v>1.37241905583313E-2</v>
+        <v>1.78465581141482E-2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1118,14 +4381,319 @@
       </c>
       <c r="B85">
         <f>AVERAGE(B75:B84)</f>
-        <v>1.7980523082383681E-2</v>
+        <v>3.770367876591238E-2</v>
       </c>
       <c r="C85">
         <f>AVERAGE(C75:C84)</f>
-        <v>4.6972367382105487E-2</v>
+        <v>8.348055071323203E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>1</v>
+      </c>
+      <c r="B91" t="s">
+        <v>2</v>
+      </c>
+      <c r="C91" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>1</v>
+      </c>
+      <c r="B92">
+        <v>7.2716735001233698E-2</v>
+      </c>
+      <c r="C92">
+        <v>0.14175836252414101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>2</v>
+      </c>
+      <c r="B93">
+        <v>0.103592529322325</v>
+      </c>
+      <c r="C93">
+        <v>0.23843350933772001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>3</v>
+      </c>
+      <c r="B94">
+        <v>0.12682245271051501</v>
+      </c>
+      <c r="C94">
+        <v>0.27992921620276001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>4</v>
+      </c>
+      <c r="B95">
+        <v>9.9130402377585206E-2</v>
+      </c>
+      <c r="C95">
+        <v>0.23707512211589701</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>5</v>
+      </c>
+      <c r="B96">
+        <v>0.120834627713059</v>
+      </c>
+      <c r="C96">
+        <v>0.26374140187835798</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>6</v>
+      </c>
+      <c r="B97">
+        <v>5.1063588836462101E-2</v>
+      </c>
+      <c r="C97">
+        <v>0.11148833614487801</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>7</v>
+      </c>
+      <c r="B98">
+        <v>0.12677107667388199</v>
+      </c>
+      <c r="C98">
+        <v>0.27479313725993498</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>8</v>
+      </c>
+      <c r="B99">
+        <v>9.9821073653700201E-2</v>
+      </c>
+      <c r="C99">
+        <v>0.21416179252013201</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>9</v>
+      </c>
+      <c r="B100">
+        <v>8.1976442102352498E-3</v>
+      </c>
+      <c r="C100">
+        <v>9.6384267161555206E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>10</v>
+      </c>
+      <c r="B101">
+        <v>0.117654678798976</v>
+      </c>
+      <c r="C101">
+        <v>0.168758686868688</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102">
+        <f>AVERAGE(B92:B101)</f>
+        <v>9.266048092979734E-2</v>
+      </c>
+      <c r="C102">
+        <f>AVERAGE(C92:C101)</f>
+        <v>0.19397779915686644</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>0</v>
+      </c>
+      <c r="B107" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>1</v>
+      </c>
+      <c r="B109" t="s">
+        <v>2</v>
+      </c>
+      <c r="C109" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>1</v>
+      </c>
+      <c r="B110">
+        <v>9.3402468402396494E-2</v>
+      </c>
+      <c r="C110">
+        <v>0.207491974297737</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>2</v>
+      </c>
+      <c r="B111">
+        <v>1.78614211984813E-2</v>
+      </c>
+      <c r="C111">
+        <v>9.8268714832012702E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>3</v>
+      </c>
+      <c r="B112">
+        <v>3.1655901457871997E-2</v>
+      </c>
+      <c r="C112">
+        <v>6.8886354453305307E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>4</v>
+      </c>
+      <c r="B113">
+        <v>9.6420958075981694E-2</v>
+      </c>
+      <c r="C113">
+        <v>0.20737843392390201</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>5</v>
+      </c>
+      <c r="B114">
+        <v>1.20872889416388E-2</v>
+      </c>
+      <c r="C114">
+        <v>2.90952467500332E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>6</v>
+      </c>
+      <c r="B115">
+        <v>2.3075143045881999E-2</v>
+      </c>
+      <c r="C115">
+        <v>3.0262377365511101E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>7</v>
+      </c>
+      <c r="B116">
+        <v>1.16090302287098E-2</v>
+      </c>
+      <c r="C116">
+        <v>1.88031895885028E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>8</v>
+      </c>
+      <c r="B117">
+        <v>3.2944637917724097E-2</v>
+      </c>
+      <c r="C117">
+        <v>9.5607879460678794E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>9</v>
+      </c>
+      <c r="B118">
+        <v>1.6378980862200399E-2</v>
+      </c>
+      <c r="C118">
+        <v>5.4809600331596202E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>10</v>
+      </c>
+      <c r="B119">
+        <v>1.84155212054853E-2</v>
+      </c>
+      <c r="C119">
+        <v>0.224378683920749</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>4</v>
+      </c>
+      <c r="B120">
+        <f>AVERAGE(B110:B119)</f>
+        <v>3.538513513363719E-2</v>
+      </c>
+      <c r="C120">
+        <f>AVERAGE(C110:C119)</f>
+        <v>0.1034982454924028</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Started writting report, need to test perfect branch one more time
</commit_message>
<xml_diff>
--- a/Test  Results.xlsx
+++ b/Test  Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="33">
   <si>
     <t>Method:</t>
   </si>
@@ -66,9 +66,6 @@
     <t>hasn't changed over multiple turns, one child in uniform, tournament select, tournament replace:</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.012728765345678653	</t>
-  </si>
-  <si>
     <t>PERFEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEEECT</t>
   </si>
   <si>
@@ -109,6 +106,18 @@
   </si>
   <si>
     <t>4 hidden nodes, 100 population,changing mutationRate if previousBest.fitness==best.fitnessand best.fitness&gt;0.017</t>
+  </si>
+  <si>
+    <t>TEST 9</t>
+  </si>
+  <si>
+    <t>ORIGINAL CW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 hidden nodes, 200 population, </t>
+  </si>
+  <si>
+    <t>replace worst, random parent selection,</t>
   </si>
 </sst>
 </file>
@@ -3644,10 +3653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V140"/>
+  <dimension ref="A1:V160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N103" workbookViewId="0">
-      <selection activeCell="U110" sqref="U110"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="M59" sqref="M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4111,7 +4120,7 @@
         <v>12</v>
       </c>
       <c r="D52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.3">
@@ -4125,13 +4134,13 @@
         <v>0</v>
       </c>
       <c r="M54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T54" t="s">
         <v>0</v>
       </c>
       <c r="U54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.3">
@@ -4210,8 +4219,8 @@
       <c r="B58">
         <v>1.06292830988239E-2</v>
       </c>
-      <c r="C58" t="s">
-        <v>15</v>
+      <c r="C58">
+        <v>1.27287653456786E-2</v>
       </c>
       <c r="L58">
         <v>2</v>
@@ -4474,7 +4483,7 @@
       </c>
       <c r="C67">
         <f>AVERAGE(C57:C66)</f>
-        <v>4.6972367382105487E-2</v>
+        <v>4.3548007178462793E-2</v>
       </c>
       <c r="L67" t="s">
         <v>4</v>
@@ -4501,7 +4510,7 @@
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.3">
@@ -4514,7 +4523,7 @@
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.3">
@@ -4653,7 +4662,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -4666,7 +4675,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -4805,7 +4814,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -4818,7 +4827,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
@@ -4957,7 +4966,7 @@
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.3">
@@ -4965,19 +4974,19 @@
         <v>0</v>
       </c>
       <c r="B127" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L127" t="s">
         <v>0</v>
       </c>
       <c r="M127" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T127" t="s">
         <v>0</v>
       </c>
       <c r="U127" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.3">
@@ -5147,7 +5156,7 @@
         <v>0.106033239470656</v>
       </c>
       <c r="D134" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L134">
         <v>5</v>
@@ -5346,6 +5355,161 @@
       <c r="V140">
         <f>AVERAGE(V130:V139)</f>
         <v>7.6595235297230641E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>29</v>
+      </c>
+      <c r="B145" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>0</v>
+      </c>
+      <c r="B147" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B148" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>1</v>
+      </c>
+      <c r="B149" t="s">
+        <v>2</v>
+      </c>
+      <c r="C149" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>1</v>
+      </c>
+      <c r="B150">
+        <v>0.13299845414636799</v>
+      </c>
+      <c r="C150">
+        <v>0.27902066547717003</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>2</v>
+      </c>
+      <c r="B151">
+        <v>0.13563810204085</v>
+      </c>
+      <c r="C151">
+        <v>0.28723236699432197</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>3</v>
+      </c>
+      <c r="B152">
+        <v>0.120337625475382</v>
+      </c>
+      <c r="C152">
+        <v>0.27564133468400798</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>4</v>
+      </c>
+      <c r="B153">
+        <v>0.17801790634224299</v>
+      </c>
+      <c r="C153">
+        <v>0.35197137499534698</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>5</v>
+      </c>
+      <c r="B154">
+        <v>0.12931036207077801</v>
+      </c>
+      <c r="C154">
+        <v>0.23684812577423101</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>6</v>
+      </c>
+      <c r="B155">
+        <v>0.20480812931675599</v>
+      </c>
+      <c r="C155">
+        <v>0.35089827423202502</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>7</v>
+      </c>
+      <c r="B156">
+        <v>9.0942183983095698E-2</v>
+      </c>
+      <c r="C156">
+        <v>0.21102485324325099</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>8</v>
+      </c>
+      <c r="B157">
+        <v>9.2871148175299095E-2</v>
+      </c>
+      <c r="C157">
+        <v>0.15266968401499001</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>9</v>
+      </c>
+      <c r="B158">
+        <v>0.116326957866423</v>
+      </c>
+      <c r="C158">
+        <v>0.29704662278780902</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>10</v>
+      </c>
+      <c r="B159">
+        <v>0.174028696284241</v>
+      </c>
+      <c r="C159">
+        <v>0.29677895377643898</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>4</v>
+      </c>
+      <c r="B160">
+        <f>AVERAGE(B150:B159)</f>
+        <v>0.13752795657014358</v>
+      </c>
+      <c r="C160">
+        <f>AVERAGE(C150:C159)</f>
+        <v>0.27391322559795916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tested again, run 30 experiments, everything is perfect, ready for the demo
</commit_message>
<xml_diff>
--- a/Test  Results.xlsx
+++ b/Test  Results.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552421A6-1AC9-4506-A55D-344BFA7EBB36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="14772"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="36">
   <si>
     <t>Method:</t>
   </si>
@@ -125,11 +131,14 @@
   <si>
     <t>Best with 7 hidden nodes</t>
   </si>
+  <si>
+    <t>7  hidden nodes, 150 population, changing mutationRate if previousBest.fitness==best.fitness and best.fitness&gt;0.017</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3652,29 +3661,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="N173" sqref="N173"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="I157" sqref="I157"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.5546875" customWidth="1"/>
-    <col min="14" max="14" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="41.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.5703125" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="41.7109375" customWidth="1"/>
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3682,7 +3691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -3693,7 +3702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3704,7 +3713,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -3715,7 +3724,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -3726,7 +3735,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -3737,7 +3746,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -3748,7 +3757,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -3759,7 +3768,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
@@ -3770,7 +3779,7 @@
         <v>0.224</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
@@ -3781,7 +3790,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9</v>
       </c>
@@ -3792,7 +3801,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -3803,7 +3812,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -3816,12 +3825,12 @@
         <v>0.15489999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -3829,7 +3838,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -3840,7 +3849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -3851,7 +3860,7 @@
         <v>0.126157978460465</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -3862,7 +3871,7 @@
         <v>6.5105006466554996E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3873,7 +3882,7 @@
         <v>0.26143750737414401</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3884,7 +3893,7 @@
         <v>0.18212223567218</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5</v>
       </c>
@@ -3895,7 +3904,7 @@
         <v>0.229379370515812</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
@@ -3906,7 +3915,7 @@
         <v>0.11164213217684101</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7</v>
       </c>
@@ -3917,7 +3926,7 @@
         <v>0.23954424544462399</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>8</v>
       </c>
@@ -3928,7 +3937,7 @@
         <v>8.5666827098220794E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9</v>
       </c>
@@ -3939,7 +3948,7 @@
         <v>0.19854631606070799</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>10</v>
       </c>
@@ -3950,7 +3959,7 @@
         <v>4.0005319956159899E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -3963,12 +3972,12 @@
         <v>0.15396069392257097</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -3976,12 +3985,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -3992,7 +4001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1</v>
       </c>
@@ -4003,7 +4012,7 @@
         <v>1.8615947712303901E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -4014,7 +4023,7 @@
         <v>0.20648204214930199</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
@@ -4025,7 +4034,7 @@
         <v>0.28718454192987503</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>4</v>
       </c>
@@ -4036,7 +4045,7 @@
         <v>1.29534540516409E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>5</v>
       </c>
@@ -4047,7 +4056,7 @@
         <v>0.15976090266479401</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>6</v>
       </c>
@@ -4058,7 +4067,7 @@
         <v>0.21344636790087601</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>7</v>
       </c>
@@ -4069,7 +4078,7 @@
         <v>0.220517778637558</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>8</v>
       </c>
@@ -4080,7 +4089,7 @@
         <v>0.12331353760710401</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>9</v>
       </c>
@@ -4091,7 +4100,7 @@
         <v>0.21776878241487299</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>10</v>
       </c>
@@ -4102,7 +4111,7 @@
         <v>0.176829354331655</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -4115,7 +4124,7 @@
         <v>0.16368727093999819</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -4123,7 +4132,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -4143,7 +4152,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>14</v>
       </c>
@@ -4154,7 +4163,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -4183,7 +4192,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1</v>
       </c>
@@ -4212,7 +4221,7 @@
         <v>6.3709956349113195E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2</v>
       </c>
@@ -4241,7 +4250,7 @@
         <v>9.1350029470918508E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>3</v>
       </c>
@@ -4270,7 +4279,7 @@
         <v>0.17822118449368499</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4</v>
       </c>
@@ -4299,7 +4308,7 @@
         <v>0.110600571939913</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>5</v>
       </c>
@@ -4328,7 +4337,7 @@
         <v>1.36690550476797E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>6</v>
       </c>
@@ -4357,7 +4366,7 @@
         <v>0.13040380958081399</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>7</v>
       </c>
@@ -4386,7 +4395,7 @@
         <v>5.8280118319736099E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>8</v>
       </c>
@@ -4415,7 +4424,7 @@
         <v>0.130405726646245</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>9</v>
       </c>
@@ -4444,7 +4453,7 @@
         <v>5.2835228950862102E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>10</v>
       </c>
@@ -4473,7 +4482,7 @@
         <v>0.121242931210404</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -4508,12 +4517,12 @@
         <v>8.1605147899778144E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -4521,12 +4530,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1</v>
       </c>
@@ -4537,7 +4546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1</v>
       </c>
@@ -4548,7 +4557,7 @@
         <v>0.110245305644407</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2</v>
       </c>
@@ -4559,7 +4568,7 @@
         <v>0.165086018359449</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>3</v>
       </c>
@@ -4570,7 +4579,7 @@
         <v>0.124602628137528</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>4</v>
       </c>
@@ -4581,7 +4590,7 @@
         <v>6.3508739254674706E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>5</v>
       </c>
@@ -4592,7 +4601,7 @@
         <v>0.12134464855332</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>6</v>
       </c>
@@ -4603,7 +4612,7 @@
         <v>3.3550771835034403E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>7</v>
       </c>
@@ -4614,7 +4623,7 @@
         <v>3.4738887039438102E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>8</v>
       </c>
@@ -4625,7 +4634,7 @@
         <v>0.13552208322409601</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>9</v>
       </c>
@@ -4636,7 +4645,7 @@
         <v>2.8359866970224999E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>10</v>
       </c>
@@ -4647,7 +4656,7 @@
         <v>1.78465581141482E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>4</v>
       </c>
@@ -4660,12 +4669,12 @@
         <v>8.348055071323203E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -4673,12 +4682,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>1</v>
       </c>
@@ -4689,7 +4698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1</v>
       </c>
@@ -4700,7 +4709,7 @@
         <v>0.14175836252414101</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2</v>
       </c>
@@ -4711,7 +4720,7 @@
         <v>0.23843350933772001</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>3</v>
       </c>
@@ -4722,7 +4731,7 @@
         <v>0.27992921620276001</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>4</v>
       </c>
@@ -4733,7 +4742,7 @@
         <v>0.23707512211589701</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>5</v>
       </c>
@@ -4744,7 +4753,7 @@
         <v>0.26374140187835798</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>6</v>
       </c>
@@ -4755,7 +4764,7 @@
         <v>0.11148833614487801</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>7</v>
       </c>
@@ -4766,7 +4775,7 @@
         <v>0.27479313725993498</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>8</v>
       </c>
@@ -4777,7 +4786,7 @@
         <v>0.21416179252013201</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>9</v>
       </c>
@@ -4788,7 +4797,7 @@
         <v>9.6384267161555206E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>10</v>
       </c>
@@ -4799,7 +4808,7 @@
         <v>0.168758686868688</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>4</v>
       </c>
@@ -4812,12 +4821,12 @@
         <v>0.19397779915686644</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>0</v>
       </c>
@@ -4825,12 +4834,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>1</v>
       </c>
@@ -4841,7 +4850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>1</v>
       </c>
@@ -4852,7 +4861,7 @@
         <v>0.207491974297737</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2</v>
       </c>
@@ -4863,7 +4872,7 @@
         <v>9.8268714832012702E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>3</v>
       </c>
@@ -4874,7 +4883,7 @@
         <v>6.8886354453305307E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>4</v>
       </c>
@@ -4885,7 +4894,7 @@
         <v>0.20737843392390201</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>5</v>
       </c>
@@ -4896,7 +4905,7 @@
         <v>2.90952467500332E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>6</v>
       </c>
@@ -4907,7 +4916,7 @@
         <v>3.0262377365511101E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>7</v>
       </c>
@@ -4918,7 +4927,7 @@
         <v>1.88031895885028E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>8</v>
       </c>
@@ -4929,7 +4938,7 @@
         <v>9.5607879460678794E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>9</v>
       </c>
@@ -4940,7 +4949,7 @@
         <v>5.4809600331596202E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>10</v>
       </c>
@@ -4951,7 +4960,7 @@
         <v>0.224378683920749</v>
       </c>
     </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>4</v>
       </c>
@@ -4964,12 +4973,12 @@
         <v>0.1034982454924028</v>
       </c>
     </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>0</v>
       </c>
@@ -4989,7 +4998,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>14</v>
       </c>
@@ -5000,7 +5009,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>1</v>
       </c>
@@ -5029,7 +5038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>1</v>
       </c>
@@ -5058,7 +5067,7 @@
         <v>0.106230496487051</v>
       </c>
     </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2</v>
       </c>
@@ -5087,7 +5096,7 @@
         <v>9.0169442947691705E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>3</v>
       </c>
@@ -5116,7 +5125,7 @@
         <v>0.216209748431546</v>
       </c>
     </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>4</v>
       </c>
@@ -5145,7 +5154,7 @@
         <v>1.36489983595472E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>5</v>
       </c>
@@ -5177,7 +5186,7 @@
         <v>0.116893070238167</v>
       </c>
     </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>6</v>
       </c>
@@ -5206,7 +5215,7 @@
         <v>8.5196891164783795E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>7</v>
       </c>
@@ -5235,7 +5244,7 @@
         <v>7.8612866470405395E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>8</v>
       </c>
@@ -5264,7 +5273,7 @@
         <v>0.129466590804975</v>
       </c>
     </row>
-    <row r="138" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>9</v>
       </c>
@@ -5293,7 +5302,7 @@
         <v>4.9779901229594699E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>10</v>
       </c>
@@ -5322,7 +5331,7 @@
         <v>2.7173128710214701E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>4</v>
       </c>
@@ -5357,7 +5366,7 @@
         <v>7.6595235297230641E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>29</v>
       </c>
@@ -5365,7 +5374,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>0</v>
       </c>
@@ -5373,12 +5382,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>1</v>
       </c>
@@ -5389,7 +5398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>1</v>
       </c>
@@ -5400,7 +5409,7 @@
         <v>0.27902066547717003</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>2</v>
       </c>
@@ -5411,7 +5420,7 @@
         <v>0.28723236699432197</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>3</v>
       </c>
@@ -5422,7 +5431,7 @@
         <v>0.27564133468400798</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>4</v>
       </c>
@@ -5433,7 +5442,7 @@
         <v>0.35197137499534698</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>5</v>
       </c>
@@ -5444,7 +5453,7 @@
         <v>0.23684812577423101</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>6</v>
       </c>
@@ -5455,7 +5464,7 @@
         <v>0.35089827423202502</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>7</v>
       </c>
@@ -5466,7 +5475,7 @@
         <v>0.21102485324325099</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>8</v>
       </c>
@@ -5477,7 +5486,7 @@
         <v>0.15266968401499001</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>9</v>
       </c>
@@ -5488,7 +5497,7 @@
         <v>0.29704662278780902</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>10</v>
       </c>
@@ -5499,7 +5508,7 @@
         <v>0.29677895377643898</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>4</v>
       </c>
@@ -5512,7 +5521,7 @@
         <v>0.27391322559795916</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>33</v>
       </c>
@@ -5520,20 +5529,20 @@
         <v>34</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>0</v>
       </c>
       <c r="B166" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>1</v>
       </c>
@@ -5544,7 +5553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>1</v>
       </c>
@@ -5555,7 +5564,7 @@
         <v>1.8140511348919999E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>2</v>
       </c>
@@ -5566,7 +5575,7 @@
         <v>1.04555978596637E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>3</v>
       </c>
@@ -5577,7 +5586,7 @@
         <v>2.9575877321937099E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>4</v>
       </c>
@@ -5588,47 +5597,83 @@
         <v>3.2473757806772099E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>5</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B173">
+        <v>1.8517606963887701E-2</v>
+      </c>
+      <c r="C173">
+        <v>2.8464791516148301E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>6</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B174">
+        <v>1.4448711495505501E-2</v>
+      </c>
+      <c r="C174">
+        <v>5.4878183472145098E-2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>7</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B175">
+        <v>1.19151623878418E-2</v>
+      </c>
+      <c r="C175">
+        <v>2.2082454632151201E-2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>8</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B176">
+        <v>7.3412015559645499E-3</v>
+      </c>
+      <c r="C176">
+        <v>8.6739115684443605E-3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>9</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B177">
+        <v>1.27229251042993E-2</v>
+      </c>
+      <c r="C177">
+        <v>1.6435165285498099E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>10</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B178">
+        <v>1.4792143935276499E-2</v>
+      </c>
+      <c r="C178">
+        <v>2.2697209339582199E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>4</v>
       </c>
       <c r="B179">
         <f>AVERAGE(B169:B178)</f>
-        <v>1.2783939085728186E-2</v>
+        <v>1.3087350778568808E-2</v>
       </c>
       <c r="C179">
         <f>AVERAGE(C169:C178)</f>
-        <v>2.2661436084323226E-2</v>
+        <v>2.4387746015126215E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>